<commit_message>
Gestion des cotisations | enregistrement de paiement avec gestion des comptes de cotisations
</commit_message>
<xml_diff>
--- a/Conception/beneficiaire.xlsx
+++ b/Conception/beneficiaire.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Nom</t>
   </si>
@@ -52,22 +52,10 @@
     <t>Masculin</t>
   </si>
   <si>
-    <t>13.05.2001</t>
-  </si>
-  <si>
-    <t>101010101010</t>
-  </si>
-  <si>
     <t>Responsable</t>
   </si>
   <si>
     <t>Membre</t>
-  </si>
-  <si>
-    <t>12.06.2020</t>
-  </si>
-  <si>
-    <t>12.02.1995</t>
   </si>
 </sst>
 </file>
@@ -75,7 +63,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.00000E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -168,7 +156,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,7 +464,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +506,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -529,22 +517,20 @@
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>13</v>
-      </c>
+      <c r="E2" s="4">
+        <v>34742</v>
+      </c>
+      <c r="F2" s="8"/>
       <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="H2" s="4">
+        <v>43263</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -555,17 +541,15 @@
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="E3" s="4">
+        <v>37024</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
+      <c r="H3" s="4">
+        <v>43994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>